<commit_message>
Neud popeth ar checklist 04/02
</commit_message>
<xml_diff>
--- a/Glossary.xlsx
+++ b/Glossary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Dysgu_Peirianyddol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FC077F2-CC04-466D-87AC-2BE9168EDEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0491B48-C2D6-4F93-ACB2-A56F7E0BBCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{34CDB60F-D79D-4AB4-9816-352E277CCA0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{34CDB60F-D79D-4AB4-9816-352E277CCA0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Glossary" sheetId="1" r:id="rId1"/>
+    <sheet name="References" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Saesneg</t>
   </si>
@@ -81,16 +82,30 @@
   </si>
   <si>
     <t>k cymydog agosaf</t>
+  </si>
+  <si>
+    <t>llun (clystyrau_k_modd)</t>
+  </si>
+  <si>
+    <t>https://h1ros.github.io/posts/k-means-clustering/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,13 +128,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E15E5D-13B1-45D6-B65F-166315656A24}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,4 +528,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF28A50-F48E-4E56-A493-7E8A5E797331}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{F8C00614-D618-40EF-8C2B-8F9634991399}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
wedi mergio sylwadau a wedi sortio conflicts
</commit_message>
<xml_diff>
--- a/Glossary.xlsx
+++ b/Glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Dysgu_Peirianyddol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BD7C29-7083-4882-93FE-379F269554E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE05BAD-70D3-4C51-9E46-7905D4922AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{34CDB60F-D79D-4AB4-9816-352E277CCA0B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Saesneg</t>
   </si>
@@ -94,6 +94,66 @@
   </si>
   <si>
     <t>https://learning.oreilly.com/library/view/Classification,+Parameter+Estimation+and+State+Estimation:+An+Engineering+Approach+Using+MATLAB/9780470090138/12_chap07.html#chap07-sec006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adnodd codio cymraeg </t>
+  </si>
+  <si>
+    <t>Adnodd data/maths uwch yn gymraeg</t>
+  </si>
+  <si>
+    <t>https://adnoddau.porth.ac.uk/webapps/portal/execute/tabs/tabAction?tab_tab_group_id=_90_1</t>
+  </si>
+  <si>
+    <t>https://projects.raspberrypi.org/cy-GB/codeclub</t>
+  </si>
+  <si>
+    <t>https://www.technocamps.com/cy/resources/python</t>
+  </si>
+  <si>
+    <t>https://github.com/meigwilym/haciaith13</t>
+  </si>
+  <si>
+    <t>https://sgiliauymchwilcyfrifiadurol.github.io/</t>
+  </si>
+  <si>
+    <t>https://llyfrgell.porth.ac.uk/View.aspx?id=1716~4p~QbzBunJu</t>
+  </si>
+  <si>
+    <t>https://github.com/porthtechnolegauiaith</t>
+  </si>
+  <si>
+    <t>http://techiaith.cymru/yr-adnoddau/llawlyfr-technolegau-iaith/</t>
+  </si>
+  <si>
+    <t>https://www.meddal.com/meddal/?page_id=1111</t>
+  </si>
+  <si>
+    <t>https://www.technocamps.com/cy/resources/arduino</t>
+  </si>
+  <si>
+    <t>https://apps.apple.com/us/app/botio/id1296278646?ls=1</t>
+  </si>
+  <si>
+    <t>https://www.technocamps.com/cy/resources/artificial-intelligence</t>
+  </si>
+  <si>
+    <t>https://www.technocamps.com/cy/resources</t>
+  </si>
+  <si>
+    <t>http://resources.hwb.wales.gov.uk/VTC/ngfl/computing/164/index.html</t>
+  </si>
+  <si>
+    <t>https://www.mathemateg.com/</t>
+  </si>
+  <si>
+    <t>https://llyfrgell.porth.ac.uk/Default.aspx?search=python&amp;pagesize=20&amp;page=2&amp;fp=0</t>
+  </si>
+  <si>
+    <t>https://llyfrgell.porth.ac.uk/View.aspx?id=5729~4x~8AS68GtY</t>
+  </si>
+  <si>
+    <t>https://adnoddau.cbac.co.uk/Pages/ResourceSingle.aspx?rIid=2660</t>
   </si>
 </sst>
 </file>
@@ -538,16 +598,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF28A50-F48E-4E56-A493-7E8A5E797331}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="178.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -566,10 +626,119 @@
         <v>19</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{F8C00614-D618-40EF-8C2B-8F9634991399}"/>
     <hyperlink ref="B2" r:id="rId2" location="chap07-sec006" display="https://learning.oreilly.com/library/view/Classification,+Parameter+Estimation+and+State+Estimation:+An+Engineering+Approach+Using+MATLAB/9780470090138/12_chap07.html - chap07-sec006" xr:uid="{45D7ABBE-8860-4491-8F74-ABAB54A3F94E}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{9B4BA9C1-BF32-4306-ABA4-9D084BBEBD20}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{45D69A79-995F-4A43-9539-5B526F831756}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{5A65EC0C-7D76-4310-85B3-A430A875898F}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{360472E4-E866-4098-AE36-48AE775497AC}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{23F89BB1-09FC-4D3A-BE6D-208D7BB87D51}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{B082446A-DAA0-4AAC-9172-A4F34EA7E306}"/>
+    <hyperlink ref="B5" r:id="rId9" xr:uid="{9FE327D1-C366-41B7-9449-9A6D906266F5}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{AE516226-86B3-4E07-BB07-7C361228CCA2}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{45E39A75-561F-4BF3-A4F8-D2BC6BF99E14}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{2EC0032A-D912-49A9-9F19-FE7AB6102C88}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{F95E26A8-4DC8-4EDA-91B7-F8114CFA98AC}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{B9A7C2B5-D6A2-4C37-BFC1-15AB68EACA9B}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{45C7C191-577D-4747-B941-05A683521C65}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{48E89424-8A14-410C-86FF-C3CAD72A4484}"/>
+    <hyperlink ref="B6" r:id="rId17" xr:uid="{423B725D-2852-4173-83A1-99F60BB3C007}"/>
+    <hyperlink ref="A18" r:id="rId18" xr:uid="{56045806-D201-4E5C-8024-FAE5A50250FA}"/>
+    <hyperlink ref="B8" r:id="rId19" xr:uid="{C12944AB-8906-406A-AECC-D38EDEC274B5}"/>
+    <hyperlink ref="B9" r:id="rId20" xr:uid="{D9D8B577-1961-4916-912E-32C8C8E5653E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>